<commit_message>
Fixed payload hardcoded values.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hoccdc-my.sharepoint.com/personal/remy_vanherweghem_parl_gc_ca/Documents/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{1586D9BE-0BEE-4142-9B86-AB9744788D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6147CED-5E31-4E82-9EB1-6A03901902FF}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{1586D9BE-0BEE-4142-9B86-AB9744788D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AA5A593-5E4A-4199-8B3A-5991456BB8FC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
@@ -540,9 +540,6 @@
     <t>warning_fr</t>
   </si>
   <si>
-    <t>2024-2025</t>
-  </si>
-  <si>
     <t>2025-2026</t>
   </si>
   <si>
@@ -1045,6 +1042,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2029-2030</t>
   </si>
 </sst>
 </file>
@@ -1467,6 +1467,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{18D3F2AD-386C-47D7-A08A-D0F9FA78FC08}" name="Table12" displayName="Table12" ref="A1:C14" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:C14" xr:uid="{18D3F2AD-386C-47D7-A08A-D0F9FA78FC08}">
@@ -1808,24 +1812,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="74" t="s">
         <v>202</v>
-      </c>
-      <c r="B1" s="74" t="s">
-        <v>204</v>
-      </c>
-      <c r="C1" s="74" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="76" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1836,7 +1840,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1847,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1858,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1866,10 +1870,10 @@
         <v>158</v>
       </c>
       <c r="B6" s="76" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1878,7 +1882,7 @@
       </c>
       <c r="B7" s="76"/>
       <c r="C7" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1887,7 +1891,7 @@
       </c>
       <c r="B8" s="76"/>
       <c r="C8" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1896,7 +1900,7 @@
       </c>
       <c r="B9" s="76"/>
       <c r="C9" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1905,7 +1909,7 @@
       </c>
       <c r="B10" s="76"/>
       <c r="C10" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1914,59 +1918,59 @@
       </c>
       <c r="B11" s="76"/>
       <c r="C11" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" s="76"/>
       <c r="C12" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B13" s="76"/>
       <c r="C13" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B14" s="76"/>
       <c r="C14" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1983,7 +1987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA5658-E2EA-4E0B-B547-2D4F388F10E4}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2002,7 +2008,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
         <v>157</v>
@@ -2032,10 +2038,10 @@
         <v>165</v>
       </c>
       <c r="K1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M1" s="75" t="s">
         <v>166</v>
@@ -2044,27 +2050,27 @@
         <v>167</v>
       </c>
       <c r="O1" s="75" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="P1" s="75" t="s">
         <v>177</v>
       </c>
       <c r="Q1" s="75" t="s">
-        <v>178</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="73" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="73" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -2074,7 +2080,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M2" s="75">
         <v>0</v>
@@ -2094,16 +2100,16 @@
     </row>
     <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" s="73" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="73" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -2113,7 +2119,7 @@
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M3" s="75">
         <v>0</v>
@@ -2136,13 +2142,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="73" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -2152,7 +2158,7 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M4" s="75">
         <f>'For user (EN)'!C6</f>
@@ -2180,13 +2186,13 @@
         <v>59</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" s="73" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -2196,7 +2202,7 @@
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M5" s="75">
         <f>'For user (EN)'!C10</f>
@@ -2221,30 +2227,30 @@
     </row>
     <row r="6" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M6" s="75">
         <f>'For user (EN)'!C12</f>
@@ -2272,13 +2278,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C7" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="73" t="s">
         <v>181</v>
-      </c>
-      <c r="D7" s="73" t="s">
-        <v>182</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -2288,7 +2294,7 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M7" s="75">
         <f>'For user (EN)'!C11</f>
@@ -2316,13 +2322,13 @@
         <v>58</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C8" s="73" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -2332,7 +2338,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M8" s="75">
         <f>'For user (EN)'!C13</f>
@@ -2360,19 +2366,19 @@
         <v>51</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="73" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="73" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>189</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>190</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -2405,22 +2411,22 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="73" t="s">
         <v>221</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="D10" s="73" t="s">
-        <v>222</v>
-      </c>
       <c r="E10" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
@@ -2456,19 +2462,19 @@
         <v>52</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -2504,19 +2510,19 @@
         <v>57</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="73" t="s">
         <v>195</v>
       </c>
-      <c r="D12" s="73" t="s">
-        <v>196</v>
-      </c>
       <c r="E12" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -2549,22 +2555,22 @@
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D13" s="79" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -2595,22 +2601,22 @@
     </row>
     <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D14" s="79" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -2641,22 +2647,22 @@
     </row>
     <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D15" s="79" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -2687,22 +2693,22 @@
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D16" s="73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -2733,22 +2739,22 @@
     </row>
     <row r="17" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17" s="79" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D17" s="73" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E17" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>224</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
@@ -2779,22 +2785,22 @@
     </row>
     <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" s="79" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D18" s="73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E18" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>224</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -2825,22 +2831,22 @@
     </row>
     <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" s="79" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D19" s="73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E19" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>224</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -2871,7 +2877,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q26" s="75" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2998,23 +3004,23 @@
       </c>
       <c r="D5" s="68">
         <f>'For user (EN)'!C5</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E5" s="68">
         <f>'For user (EN)'!D5</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F5" s="68">
         <f>'For user (EN)'!E5</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G5" s="68">
         <f>'For user (EN)'!F5</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H5" s="68">
         <f>'For user (EN)'!G5</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -3130,7 +3136,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>31</v>
@@ -3159,7 +3165,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B13" s="36" t="s">
         <v>31</v>
@@ -3188,7 +3194,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B14" s="36" t="s">
         <v>31</v>
@@ -3293,7 +3299,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B18" s="36" t="s">
         <v>28</v>
@@ -3323,7 +3329,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>29</v>
@@ -3352,7 +3358,7 @@
     </row>
     <row r="20" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>30</v>
@@ -3381,10 +3387,10 @@
     </row>
     <row r="21" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="9">
@@ -3432,7 +3438,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B24" s="36" t="s">
         <v>132</v>
@@ -3461,7 +3467,7 @@
     </row>
     <row r="25" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B25" s="36" t="s">
         <v>133</v>
@@ -3490,7 +3496,7 @@
     </row>
     <row r="26" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B26" s="36" t="s">
         <v>133</v>
@@ -3519,7 +3525,7 @@
     </row>
     <row r="27" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>133</v>
@@ -3548,10 +3554,10 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="9">
@@ -3641,10 +3647,10 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="67">
@@ -3670,10 +3676,10 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="67">
@@ -3699,10 +3705,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B33" s="36" t="s">
         <v>241</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>242</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="67">
@@ -4031,7 +4037,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D3" t="s">
         <v>76</v>
@@ -4091,7 +4097,7 @@
         <v>94</v>
       </c>
       <c r="W3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -4222,83 +4228,83 @@
       </c>
       <c r="D6" s="68">
         <f>'For user (EN)'!C5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="E6" s="68">
         <f>'For user (EN)'!C5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F6" s="68">
         <f>'For user (EN)'!C5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="G6" s="68">
         <f>'For user (EN)'!C5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="H6" s="68">
         <f>'For user (EN)'!D5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="I6" s="68">
         <f>'For user (EN)'!$D5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="J6" s="68">
         <f>'For user (EN)'!$D5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="K6" s="68">
         <f>'For user (EN)'!$D5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="L6" s="4">
         <f>'For user (EN)'!$E5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="M6" s="4">
         <f>'For user (EN)'!$E5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="N6" s="4">
         <f>'For user (EN)'!$E5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="O6" s="4">
         <f>'For user (EN)'!$E5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="P6" s="4">
         <f>'For user (EN)'!$F5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="4">
         <f>'For user (EN)'!$F5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="R6" s="4">
         <f>'For user (EN)'!$F5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="S6" s="4">
         <f>'For user (EN)'!$F5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="T6" s="4">
         <f>'For user (EN)'!$G5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="U6" s="4">
         <f>'For user (EN)'!$G5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="V6" s="4">
         <f>'For user (EN)'!$G5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="W6" s="4">
         <f>'For user (EN)'!$G5/4</f>
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -4624,7 +4630,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B13" s="36" t="s">
         <v>31</v>
@@ -4713,7 +4719,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B14" s="36" t="s">
         <v>31</v>
@@ -4802,7 +4808,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>31</v>
@@ -5032,7 +5038,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>28</v>
@@ -5121,7 +5127,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>29</v>
@@ -5210,7 +5216,7 @@
     </row>
     <row r="21" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B21" s="36" t="s">
         <v>30</v>
@@ -5299,10 +5305,10 @@
     </row>
     <row r="22" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="9">
@@ -5440,7 +5446,7 @@
     </row>
     <row r="25" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B25" s="36" t="s">
         <v>130</v>
@@ -5529,7 +5535,7 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B26" s="36"/>
       <c r="C26" s="30"/>
@@ -5616,7 +5622,7 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B27" s="36"/>
       <c r="C27" s="30"/>
@@ -5703,10 +5709,10 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="B28" s="36" t="s">
         <v>300</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>301</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="9">
@@ -5792,10 +5798,10 @@
     </row>
     <row r="29" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="69">
@@ -5881,10 +5887,10 @@
     </row>
     <row r="30" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="69">
@@ -5970,10 +5976,10 @@
     </row>
     <row r="31" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="69">
@@ -6148,10 +6154,10 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="69">
@@ -6237,10 +6243,10 @@
     </row>
     <row r="34" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="69">
@@ -6326,10 +6332,10 @@
     </row>
     <row r="35" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="69">
@@ -6415,10 +6421,10 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="B36" s="36" t="s">
         <v>308</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>309</v>
       </c>
       <c r="C36" s="30"/>
       <c r="D36" s="9">
@@ -6504,10 +6510,10 @@
     </row>
     <row r="37" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="69">
@@ -6593,10 +6599,10 @@
     </row>
     <row r="38" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="69">
@@ -6682,10 +6688,10 @@
     </row>
     <row r="39" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="69">
@@ -6771,10 +6777,10 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="69">
@@ -6949,10 +6955,10 @@
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C42" s="30"/>
       <c r="D42" s="67">
@@ -7038,10 +7044,10 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C43" s="30"/>
       <c r="D43" s="67">
@@ -7127,10 +7133,10 @@
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="67">
@@ -7216,7 +7222,7 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B45" s="36" t="s">
         <v>140</v>
@@ -7305,10 +7311,10 @@
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C46" s="30"/>
       <c r="D46" s="67">
@@ -7394,10 +7400,10 @@
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="67">
@@ -7483,10 +7489,10 @@
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" s="36" t="s">
         <v>241</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>242</v>
       </c>
       <c r="C48" s="30"/>
       <c r="D48" s="67">
@@ -7713,10 +7719,10 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C52" s="30"/>
       <c r="D52" s="30"/>
@@ -7799,10 +7805,10 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
@@ -7882,10 +7888,10 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C54" s="30"/>
       <c r="D54" s="30"/>
@@ -7959,10 +7965,10 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="46"/>
@@ -8048,7 +8054,7 @@
         <v>126</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C56" s="30"/>
       <c r="D56" s="46"/>
@@ -8113,7 +8119,7 @@
         <v>127</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C57" s="30"/>
       <c r="D57" s="46"/>
@@ -8166,7 +8172,7 @@
         <v>128</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C58" s="30"/>
       <c r="D58" s="46"/>
@@ -8284,10 +8290,10 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>328</v>
       </c>
       <c r="C61" s="30"/>
       <c r="D61" s="32">
@@ -8373,10 +8379,10 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C62" s="30"/>
       <c r="D62" s="32">
@@ -8462,10 +8468,10 @@
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C63" s="30"/>
       <c r="D63" s="32">
@@ -8551,10 +8557,10 @@
     </row>
     <row r="64" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B64" s="36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C64" s="30"/>
       <c r="D64" s="32">
@@ -8640,10 +8646,10 @@
     </row>
     <row r="65" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C65" s="30"/>
       <c r="D65" s="32">
@@ -8729,7 +8735,7 @@
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B66" s="36" t="s">
         <v>148</v>
@@ -8907,7 +8913,7 @@
     </row>
     <row r="68" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A68" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B68" s="36" t="s">
         <v>146</v>
@@ -9498,7 +9504,7 @@
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D79" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E79" s="18"/>
       <c r="F79" s="18"/>
@@ -9552,9 +9558,7 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9625,11 +9629,26 @@
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="C4" s="4">
+        <f>machine_readable!M2</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <f>machine_readable!N2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <f>machine_readable!O2</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <f>machine_readable!P2</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <f>machine_readable!Q2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -9639,19 +9658,24 @@
         <v>5</v>
       </c>
       <c r="C5" s="4">
-        <v>1000</v>
+        <f>machine_readable!M3</f>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
-        <v>1000</v>
+        <f>machine_readable!N3</f>
+        <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>1000</v>
+        <f>machine_readable!O3</f>
+        <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>1000</v>
+        <f>machine_readable!P3</f>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>1000</v>
+        <f>machine_readable!Q3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -9992,7 +10016,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G6" s="62" t="s">
         <v>120</v>
@@ -10016,10 +10040,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" t="s">
         <v>282</v>
-      </c>
-      <c r="C7" t="s">
-        <v>283</v>
       </c>
       <c r="F7" s="62"/>
       <c r="H7" s="65"/>
@@ -10029,7 +10053,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B8" s="20">
         <v>0.14799999999999999</v>
@@ -10049,7 +10073,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B9" s="20">
         <v>0.496</v>
@@ -10069,7 +10093,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B10" s="20">
         <v>0.17799999999999999</v>
@@ -10089,7 +10113,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B11" s="20">
         <v>0.17799999999999999</v>
@@ -10108,7 +10132,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B12" s="77">
         <f>SUMPRODUCT(B8:B11,C8:C11)</f>
@@ -10732,7 +10756,7 @@
         <v>112</v>
       </c>
       <c r="G43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H43" t="s">
         <v>113</v>
@@ -11749,7 +11773,7 @@
     </row>
     <row r="20" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C20" s="24">
         <f>AVERAGE(C36:F36)</f>
@@ -11794,7 +11818,7 @@
     </row>
     <row r="21" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C21" s="24">
         <f t="shared" ref="C21:C22" si="16">AVERAGE(C37:F37)</f>
@@ -11839,7 +11863,7 @@
     </row>
     <row r="22" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C22" s="24">
         <f t="shared" si="16"/>
@@ -11928,7 +11952,7 @@
     </row>
     <row r="25" spans="1:82" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C25" s="49">
         <f>C$2*C16+C$3*C17+C$4*C$7*C$20+C$4*C$8*C$21+C$4*C$9*C$22</f>
@@ -12621,10 +12645,10 @@
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C36">
         <v>2.4326666666666599</v>
@@ -12734,10 +12758,10 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C37">
         <v>2.4326666666666599</v>
@@ -12847,10 +12871,10 @@
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C38">
         <v>2.4326666666666599</v>
@@ -12960,7 +12984,7 @@
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O40" s="20">
         <f>F3</f>
@@ -13065,7 +13089,7 @@
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O41" s="20">
         <f>F2</f>
@@ -13170,7 +13194,7 @@
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O42" s="20">
         <f>F4*F7</f>
@@ -13275,7 +13299,7 @@
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O43" s="20">
         <f>F4*F8</f>
@@ -13380,7 +13404,7 @@
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O44" s="20">
         <f>F4*F9</f>
@@ -13488,7 +13512,7 @@
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O46" s="24">
         <f>O33*O40+SUMPRODUCT(O35:O38,O41:O44)</f>
@@ -13627,7 +13651,7 @@
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O48" s="71">
         <f>O41*SUM(Decomposition!$B$8:$B$9)</f>
@@ -13732,7 +13756,7 @@
     </row>
     <row r="49" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O49" s="71">
         <f>O41*Decomposition!$B$10</f>
@@ -13837,7 +13861,7 @@
     </row>
     <row r="50" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O50" s="71">
         <f>O41*Decomposition!$B$11</f>
@@ -14355,13 +14379,13 @@
         <v>17</v>
       </c>
       <c r="N78" t="s">
+        <v>257</v>
+      </c>
+      <c r="O78" t="s">
         <v>258</v>
       </c>
-      <c r="O78" t="s">
+      <c r="P78" t="s">
         <v>259</v>
-      </c>
-      <c r="P78" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed payload hardcoded values x2.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hoccdc-my.sharepoint.com/personal/remy_vanherweghem_parl_gc_ca/Documents/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{1586D9BE-0BEE-4142-9B86-AB9744788D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AA5A593-5E4A-4199-8B3A-5991456BB8FC}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{1586D9BE-0BEE-4142-9B86-AB9744788D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82F3DB11-B1AB-4949-9569-AEF52CB93DB1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
   <sheets>
     <sheet name="How to interface with Web tool" sheetId="8" r:id="rId1"/>
@@ -1988,7 +1988,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9558,7 +9558,9 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9686,18 +9688,23 @@
         <v>5</v>
       </c>
       <c r="C6" s="68">
+        <f t="shared" ref="C6:G6" si="2">C4-C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="68">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E6" s="68">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F6" s="68">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G6" s="68">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed broken functions in excel file.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hoccdc-my.sharepoint.com/personal/remy_vanherweghem_parl_gc_ca/Documents/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{277030AF-9D42-4CAB-874E-E19592415F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{277030AF-9D42-4CAB-874E-E19592415F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E1B38D7-C58A-4351-96F7-5FA85BC716C1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
@@ -1921,7 +1921,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,7 +1936,8 @@
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="12" width="25.7109375" customWidth="1"/>
-    <col min="13" max="15" width="9.140625" style="75"/>
+    <col min="13" max="13" width="13.7109375" style="75" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="75"/>
     <col min="16" max="16" width="14.5703125" style="75" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="75"/>
   </cols>
@@ -2020,30 +2021,7 @@
       <c r="L2" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="M2" s="75">
-        <f>'For user (EN)'!C4</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="75">
-        <f>'For user (EN)'!D4</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="75">
-        <f>'For user (EN)'!E4</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="75">
-        <f>'For user (EN)'!F4</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" s="75">
-        <f>'For user (EN)'!G4</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="75">
-        <f>'For user (EN)'!H4</f>
-        <v>0</v>
-      </c>
+      <c r="R2" s="75"/>
     </row>
     <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2068,30 +2046,7 @@
       <c r="L3" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="M3" s="75">
-        <f>'For user (EN)'!C5</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="75">
-        <f>'For user (EN)'!D5</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="75">
-        <f>'For user (EN)'!E5</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="75">
-        <f>'For user (EN)'!F5</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="75">
-        <f>'For user (EN)'!G5</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="75">
-        <f>'For user (EN)'!H5</f>
-        <v>0</v>
-      </c>
+      <c r="R3" s="75"/>
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -2914,7 +2869,7 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10058,7 +10013,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10139,12 +10094,30 @@
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="C4" s="4">
+        <f>machine_readable!M2</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <f>machine_readable!N2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <f>machine_readable!O2</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <f>machine_readable!P2</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <f>machine_readable!Q2</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <f>machine_readable!R2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -10153,12 +10126,30 @@
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="C5" s="4">
+        <f>machine_readable!M3</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <f>machine_readable!N3</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <f>machine_readable!O3</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <f>machine_readable!P3</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <f>machine_readable!Q3</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>machine_readable!R3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">

</xml_diff>